<commit_message>
cn-#14 add padding to DataTable output
</commit_message>
<xml_diff>
--- a/test/Cactus.ExcelConverterTest/Features/DataGrid.xlsx
+++ b/test/Cactus.ExcelConverterTest/Features/DataGrid.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\itu\Cactus.net\test\Cactus.ExcelConverterTest\Features\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27EC27B0-49AD-417E-8366-1B0506D3B093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CAEBC3-0964-4CED-84D6-33828BB51417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31920" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddTwoNumbers" sheetId="1" r:id="rId1"/>
@@ -36,18 +36,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Second Number</t>
-  </si>
-  <si>
-    <t>First Number</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>I have following two numbers</t>
   </si>
   <si>
     <t>Given</t>
+  </si>
+  <si>
+    <t>First #</t>
+  </si>
+  <si>
+    <t>Second #</t>
+  </si>
+  <si>
+    <t>Op</t>
+  </si>
+  <si>
+    <t>Plus</t>
+  </si>
+  <si>
+    <t>Minus</t>
   </si>
 </sst>
 </file>
@@ -365,48 +374,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>50</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4">
-        <v>100</v>
-      </c>
-      <c r="C4">
+        <v>1000000000</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4">
         <v>200</v>
       </c>
     </row>

</xml_diff>